<commit_message>
new loadtimeseries and bugs corrected
</commit_message>
<xml_diff>
--- a/SCOPE_v1.73/input_data.xlsx
+++ b/SCOPE_v1.73/input_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects Python\SCOPE-CvT\SCOPE_v1.73\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm_projects\SCOPE-CvT\SCOPE_v1.73\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B55ACB1-5755-4436-9915-531A5BBB76B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8892" windowHeight="5196" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -17,12 +18,20 @@
     <sheet name="filenames" sheetId="3" r:id="rId3"/>
     <sheet name="inputdata" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="374">
   <si>
     <t>Cab</t>
   </si>
@@ -301,30 +310,6 @@
   </si>
   <si>
     <t>FLEX-S3_std.atm</t>
-  </si>
-  <si>
-    <t>t_.dat</t>
-  </si>
-  <si>
-    <t>year_.dat</t>
-  </si>
-  <si>
-    <t>Rin_.dat</t>
-  </si>
-  <si>
-    <t>Rli_.dat</t>
-  </si>
-  <si>
-    <t>p_.dat</t>
-  </si>
-  <si>
-    <t>Ta_.dat</t>
-  </si>
-  <si>
-    <t>ea_.dat</t>
-  </si>
-  <si>
-    <t>u_.dat</t>
   </si>
   <si>
     <t>optional_(leave_empty_for_constant_values_from_inputdata_sheet)</t>
@@ -766,12 +751,6 @@
     <t>within canopy layer resistance</t>
   </si>
   <si>
-    <t>Julian day (decimal) of start of simulations</t>
-  </si>
-  <si>
-    <t>Julian day (decimal) of end of simulations</t>
-  </si>
-  <si>
     <t>decimal deg</t>
   </si>
   <si>
@@ -1259,23 +1238,191 @@
     <t>BSMBrightness</t>
   </si>
   <si>
+    <t>LIDF_file</t>
+  </si>
+  <si>
+    <t>TIMESTAMP_START as YYYYMMDDHHMM or YYYYMMDD will  be converted automatically to doy and filtered to startDOY, endDOY from 'inputdata' sheet</t>
+  </si>
+  <si>
+    <t>RH</t>
+  </si>
+  <si>
+    <t>ec_file_berkeley</t>
+  </si>
+  <si>
+    <t>ts_input.csv</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>kPa or hPa</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>% or fraction</t>
+  </si>
+  <si>
+    <t>shortwave incoming radiation</t>
+  </si>
+  <si>
+    <t>longwave incoming radiation</t>
+  </si>
+  <si>
+    <t>wind speed</t>
+  </si>
+  <si>
+    <t>measurement height</t>
+  </si>
+  <si>
+    <t>maximum carboxylation capacity</t>
+  </si>
+  <si>
+    <t>atmospherc vapor pressure</t>
+  </si>
+  <si>
+    <t>if not present - calculated from RH_file: RH * satvap(Ta)</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>missing values are -9999, NA or N/A</t>
+  </si>
+  <si>
+    <t>f_date</t>
+  </si>
+  <si>
+    <t>interpolation_csv</t>
+  </si>
+  <si>
+    <t>values from `interpolation_csv` will be linearly interpolated to timestamp (t) of ec_file_berkeley</t>
+  </si>
+  <si>
+    <t>BSM</t>
+  </si>
+  <si>
+    <t>Meteo</t>
+  </si>
+  <si>
+    <t>Biochemistry</t>
+  </si>
+  <si>
+    <t>Leaf</t>
+  </si>
+  <si>
+    <t>relative humidity (for calculation of ea)</t>
+  </si>
+  <si>
+    <t>optiona_leaf_inclination_distribution_dat_file_with_13_rows_(probability_histogram)._MUST_be_located_in_../data/leafangles/</t>
+  </si>
+  <si>
+    <t>verification_dir</t>
+  </si>
+  <si>
+    <t>Variables below are COLUMN NAMES in time_series_files (ec_file_berkeley, interpolation_csv)</t>
+  </si>
+  <si>
+    <r>
+      <t>this is a suffix to 'dataset', so final dataset_dir is '../data/input/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dataset {Dataset_dir}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{ec_file_berkeley}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <r>
+      <t>output folder to which compare the timeseires run if</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> options.verify == 1</t>
+    </r>
+  </si>
+  <si>
+    <t>if not present - calculated from t, timezn, LAT, LON</t>
+  </si>
+  <si>
+    <t>only for ea calculations</t>
+  </si>
+  <si>
+    <t>[OPTIONAL] if provided - optional parameters (below) will be taken from this file else - from ec_file_berkeley</t>
+  </si>
+  <si>
+    <t>timestamp start YYYYMMDD[HHMMSS]</t>
+  </si>
+  <si>
+    <t>timestamp end YYYYMMDD[HHMMSS]</t>
+  </si>
+  <si>
     <t>verification_run</t>
   </si>
   <si>
-    <t>LIDF_file</t>
-  </si>
-  <si>
-    <t>optiona_leaf_inclination_distribution_file_with_3_headerlines._MUST_be_located_in_../data/leafangles/</t>
-  </si>
-  <si>
-    <t>optional_(leave_empty_for_calculations_based_on_t_file_year_timezn)</t>
+    <t>verificationdata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1413,15 +1560,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1612,7 +1750,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1710,7 +1848,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1813,6 +1952,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1848,6 +2004,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2023,7 +2196,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J96"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0"/>
@@ -2046,57 +2219,57 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -2104,7 +2277,7 @@
         <v>82</v>
       </c>
       <c r="C18" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -2112,7 +2285,7 @@
         <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -2120,7 +2293,7 @@
         <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -2128,7 +2301,7 @@
         <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -2141,7 +2314,7 @@
         <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -2149,7 +2322,7 @@
         <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -2157,7 +2330,7 @@
         <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -2165,7 +2338,7 @@
         <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -2173,7 +2346,7 @@
         <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -2181,7 +2354,7 @@
         <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -2189,7 +2362,7 @@
         <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -2197,7 +2370,7 @@
         <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -2205,12 +2378,12 @@
         <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -2218,7 +2391,7 @@
         <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -2226,7 +2399,7 @@
         <v>60</v>
       </c>
       <c r="C36" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -2237,17 +2410,17 @@
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="C39" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -2255,7 +2428,7 @@
         <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -2263,7 +2436,7 @@
         <v>70</v>
       </c>
       <c r="C43" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -2271,7 +2444,7 @@
         <v>71</v>
       </c>
       <c r="C44" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -2279,7 +2452,7 @@
         <v>72</v>
       </c>
       <c r="C45" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -2287,7 +2460,7 @@
         <v>73</v>
       </c>
       <c r="C46" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -2295,48 +2468,48 @@
         <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="37" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="14" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="36" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="52" t="s">
-        <v>128</v>
-      </c>
-      <c r="B56" s="52" t="s">
-        <v>108</v>
-      </c>
-      <c r="C56" s="52" t="s">
-        <v>109</v>
+      <c r="A56" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="53" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="53"/>
-      <c r="B57" s="53"/>
-      <c r="C57" s="53"/>
+      <c r="A57" s="54"/>
+      <c r="B57" s="54"/>
+      <c r="C57" s="54"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B58" s="11">
         <v>1</v>
@@ -2347,7 +2520,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B59" s="11">
         <v>-1</v>
@@ -2358,7 +2531,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B60" s="11">
         <v>0</v>
@@ -2369,7 +2542,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B61" s="11">
         <v>0</v>
@@ -2380,7 +2553,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B62" s="11">
         <v>-0.35</v>
@@ -2391,7 +2564,7 @@
     </row>
     <row r="63" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B63" s="12">
         <v>0</v>
@@ -2402,61 +2575,61 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="36" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="15"/>
       <c r="B68" s="16"/>
-      <c r="C68" s="54" t="s">
-        <v>235</v>
-      </c>
-      <c r="D68" s="55"/>
-      <c r="E68" s="55"/>
-      <c r="F68" s="55"/>
-      <c r="G68" s="56"/>
+      <c r="C68" s="55" t="s">
+        <v>225</v>
+      </c>
+      <c r="D68" s="56"/>
+      <c r="E68" s="56"/>
+      <c r="F68" s="56"/>
+      <c r="G68" s="57"/>
       <c r="H68" s="17"/>
       <c r="I68" s="17"/>
       <c r="J68" s="18"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="19" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B69" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D69" s="22" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="E69" s="22" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="F69" s="22" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="G69" s="23" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="H69" s="22" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="I69" s="22" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="J69" s="23" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="24" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C70" s="25">
         <v>0.2</v>
@@ -2485,10 +2658,10 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="24" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C71" s="25">
         <v>0.2</v>
@@ -2517,10 +2690,10 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C72" s="25">
         <v>0.2</v>
@@ -2549,10 +2722,10 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="24" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C73" s="25">
         <v>0.2</v>
@@ -2581,10 +2754,10 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="24" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C74" s="25">
         <v>0.2</v>
@@ -2613,10 +2786,10 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="24" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="C75" s="25">
         <v>0.2</v>
@@ -2645,10 +2818,10 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C76" s="25">
         <v>0.2</v>
@@ -2677,10 +2850,10 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="24" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C77" s="25">
         <v>0.2</v>
@@ -2709,10 +2882,10 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="24" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C78" s="25">
         <v>0.2</v>
@@ -2741,10 +2914,10 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="24" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C79" s="25">
         <v>0.2</v>
@@ -2773,10 +2946,10 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="24" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C80" s="25">
         <v>0.2</v>
@@ -2805,10 +2978,10 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="24" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C81" s="25">
         <v>0.2</v>
@@ -2837,10 +3010,10 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="31" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B82" s="32" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="C82" s="33">
         <v>0.2</v>
@@ -2869,7 +3042,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="36" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
@@ -2877,30 +3050,30 @@
         <v>75</v>
       </c>
       <c r="B86" s="41" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="C86" s="41" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D86" s="41" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="E86" s="41" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="F86" s="41" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="39" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="B87" s="39" t="s">
         <v>11</v>
       </c>
       <c r="C87" s="39" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D87" s="42">
         <v>1000</v>
@@ -2915,13 +3088,13 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="39" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="B88" s="39" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C88" s="39" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D88" s="42">
         <v>209</v>
@@ -2936,13 +3109,13 @@
     </row>
     <row r="89" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A89" s="39" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="B89" s="39" t="s">
         <v>21</v>
       </c>
       <c r="C89" s="39" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="D89" s="43">
         <v>1.4999999999999999E-2</v>
@@ -2957,13 +3130,13 @@
     </row>
     <row r="90" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A90" s="39" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="B90" s="39" t="s">
         <v>17</v>
       </c>
       <c r="C90" s="39" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="D90" s="43">
         <v>7</v>
@@ -2978,34 +3151,34 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="39" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="B91" s="39" t="s">
         <v>12</v>
       </c>
       <c r="C91" s="39" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D91" s="42" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E91" s="42" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="F91" s="42" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="G91" s="42"/>
     </row>
     <row r="92" spans="1:10" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A92" s="39" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="B92" s="39" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="C92" s="39" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D92" s="42">
         <v>380</v>
@@ -3017,18 +3190,18 @@
         <v>500</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A93" s="39" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="C93" s="39" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="D93" s="42" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="E93" s="42">
         <v>0</v>
@@ -3039,13 +3212,13 @@
     </row>
     <row r="94" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A94" s="39" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="B94" s="39" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="C94" s="39" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="D94" s="42">
         <v>1</v>
@@ -3059,13 +3232,13 @@
     </row>
     <row r="95" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A95" s="44" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="B95" s="44" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C95" s="44" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="D95" s="45">
         <v>0</v>
@@ -3079,13 +3252,13 @@
     </row>
     <row r="96" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="46" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="B96" s="46" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C96" s="46" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="D96" s="47">
         <v>1</v>
@@ -3111,11 +3284,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3131,7 +3304,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -3139,7 +3312,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>88</v>
@@ -3153,10 +3326,10 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -3164,10 +3337,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3175,10 +3348,10 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -3186,10 +3359,10 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E9" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -3197,10 +3370,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="E10" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -3208,10 +3381,10 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E11" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -3219,10 +3392,10 @@
         <v>0</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E12" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -3230,10 +3403,10 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E13" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -3241,10 +3414,10 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="E14" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -3252,10 +3425,10 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="E15" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -3263,10 +3436,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E16" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -3274,10 +3447,10 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E17" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -3285,7 +3458,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="E18" t="s">
         <v>48</v>
@@ -3293,29 +3466,29 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
         <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="E20" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="s">
         <v>47</v>
@@ -3326,24 +3499,24 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
         <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="E23" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3354,56 +3527,59 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:DV58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" customWidth="1"/>
+    <col min="13" max="13" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -3411,150 +3587,557 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="N9" s="49"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>362</v>
       </c>
       <c r="B11" t="s">
+        <v>373</v>
+      </c>
+      <c r="D11" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>336</v>
+      </c>
+      <c r="B12" t="s">
+        <v>337</v>
+      </c>
+      <c r="D12" t="s">
+        <v>352</v>
+      </c>
+      <c r="E12" s="50"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>354</v>
+      </c>
+      <c r="D14" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D16" t="s">
+        <v>339</v>
+      </c>
+      <c r="E16" t="s">
+        <v>350</v>
+      </c>
+      <c r="F16" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>338</v>
+      </c>
+      <c r="B17" t="s">
+        <v>353</v>
+      </c>
+      <c r="E17" t="s">
+        <v>365</v>
+      </c>
+      <c r="F17" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>340</v>
+      </c>
+      <c r="E20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>341</v>
+      </c>
+      <c r="E21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E22" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>177</v>
+      </c>
+      <c r="E23" t="s">
+        <v>348</v>
+      </c>
+      <c r="F23" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>335</v>
+      </c>
+      <c r="D24" t="s">
+        <v>342</v>
+      </c>
+      <c r="E24" t="s">
+        <v>360</v>
+      </c>
+      <c r="F24" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" t="s">
+        <v>201</v>
+      </c>
+      <c r="E26" t="s">
+        <v>202</v>
+      </c>
+      <c r="F26" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="48" t="s">
+        <v>309</v>
+      </c>
+      <c r="D31" t="s">
+        <v>136</v>
+      </c>
+      <c r="E31" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>142</v>
+      </c>
+      <c r="E34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>319</v>
+      </c>
+      <c r="D35" t="s">
+        <v>136</v>
+      </c>
+      <c r="E35" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="36" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>144</v>
+      </c>
+      <c r="E36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A38" s="50" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="39" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="D39" t="s">
+        <v>342</v>
+      </c>
+      <c r="E39" t="s">
+        <v>164</v>
+      </c>
+      <c r="F39" s="50"/>
+      <c r="AA39" s="4"/>
+      <c r="AZ39" s="4"/>
+      <c r="BY39" s="4"/>
+      <c r="CX39" s="4"/>
+    </row>
+    <row r="40" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>332</v>
+      </c>
+      <c r="E40" t="s">
+        <v>329</v>
+      </c>
+      <c r="AA40" s="4"/>
+      <c r="AZ40" s="4"/>
+      <c r="BY40" s="4"/>
+      <c r="CX40" s="4"/>
+    </row>
+    <row r="41" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>327</v>
+      </c>
+      <c r="E41" t="s">
+        <v>330</v>
+      </c>
+      <c r="AA41" s="4"/>
+      <c r="AZ41" s="4"/>
+      <c r="BY41" s="4"/>
+      <c r="CX41" s="4"/>
+    </row>
+    <row r="42" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E42" t="s">
+        <v>331</v>
+      </c>
+      <c r="AA42" s="4"/>
+      <c r="AZ42" s="4"/>
+      <c r="BY42" s="4"/>
+      <c r="CX42" s="4"/>
+    </row>
+    <row r="44" spans="1:126" s="52" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="D45" t="s">
+        <v>165</v>
+      </c>
+      <c r="E45" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA45" s="4"/>
+      <c r="AB45" s="4"/>
+      <c r="AC45" s="4"/>
+      <c r="AD45" s="4"/>
+      <c r="AE45" s="4"/>
+      <c r="AF45" s="4"/>
+      <c r="AG45" s="4"/>
+      <c r="AH45" s="4"/>
+      <c r="AI45" s="4"/>
+      <c r="AJ45" s="4"/>
+      <c r="AK45" s="4"/>
+      <c r="AL45" s="4"/>
+      <c r="AM45" s="4"/>
+      <c r="AN45" s="4"/>
+      <c r="AO45" s="4"/>
+      <c r="AP45" s="4"/>
+      <c r="AQ45" s="4"/>
+      <c r="AR45" s="4"/>
+      <c r="AS45" s="4"/>
+      <c r="AT45" s="4"/>
+      <c r="AU45" s="4"/>
+      <c r="AV45" s="4"/>
+      <c r="AW45" s="4"/>
+      <c r="AX45" s="4"/>
+      <c r="AY45" s="4"/>
+      <c r="AZ45" s="4"/>
+      <c r="BA45" s="4"/>
+      <c r="BB45" s="4"/>
+      <c r="BC45" s="4"/>
+      <c r="BD45" s="4"/>
+      <c r="BE45" s="4"/>
+      <c r="BF45" s="4"/>
+      <c r="BG45" s="4"/>
+      <c r="BH45" s="4"/>
+      <c r="BI45" s="4"/>
+      <c r="BJ45" s="4"/>
+      <c r="BK45" s="4"/>
+      <c r="BL45" s="4"/>
+      <c r="BM45" s="4"/>
+      <c r="BN45" s="4"/>
+      <c r="BO45" s="4"/>
+      <c r="BP45" s="4"/>
+      <c r="BQ45" s="4"/>
+      <c r="BR45" s="4"/>
+      <c r="BS45" s="4"/>
+      <c r="BT45" s="4"/>
+      <c r="BU45" s="4"/>
+      <c r="BV45" s="4"/>
+      <c r="BW45" s="4"/>
+      <c r="BX45" s="4"/>
+      <c r="BY45" s="4"/>
+      <c r="BZ45" s="4"/>
+      <c r="CA45" s="4"/>
+      <c r="CB45" s="4"/>
+      <c r="CC45" s="4"/>
+      <c r="CD45" s="4"/>
+      <c r="CE45" s="4"/>
+      <c r="CF45" s="4"/>
+      <c r="CG45" s="4"/>
+      <c r="CH45" s="4"/>
+      <c r="CI45" s="4"/>
+      <c r="CJ45" s="4"/>
+      <c r="CK45" s="4"/>
+      <c r="CL45" s="4"/>
+      <c r="CM45" s="4"/>
+      <c r="CN45" s="4"/>
+      <c r="CO45" s="4"/>
+      <c r="CP45" s="4"/>
+      <c r="CQ45" s="4"/>
+      <c r="CR45" s="4"/>
+      <c r="CS45" s="4"/>
+      <c r="CT45" s="4"/>
+      <c r="CU45" s="4"/>
+      <c r="CV45" s="4"/>
+      <c r="CW45" s="4"/>
+      <c r="CX45" s="4"/>
+      <c r="CY45" s="4"/>
+      <c r="CZ45" s="4"/>
+      <c r="DA45" s="4"/>
+      <c r="DB45" s="4"/>
+      <c r="DC45" s="4"/>
+      <c r="DD45" s="4"/>
+      <c r="DE45" s="4"/>
+      <c r="DF45" s="4"/>
+      <c r="DG45" s="4"/>
+      <c r="DH45" s="4"/>
+      <c r="DI45" s="4"/>
+      <c r="DJ45" s="4"/>
+      <c r="DK45" s="4"/>
+      <c r="DL45" s="4"/>
+      <c r="DM45" s="4"/>
+      <c r="DN45" s="4"/>
+      <c r="DO45" s="4"/>
+      <c r="DP45" s="4"/>
+      <c r="DQ45" s="4"/>
+      <c r="DR45" s="4"/>
+      <c r="DS45" s="4"/>
+      <c r="DT45" s="4"/>
+      <c r="DU45" s="4"/>
+      <c r="DV45" s="4"/>
+    </row>
+    <row r="46" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" t="s">
+        <v>167</v>
+      </c>
+      <c r="AA46" s="4"/>
+      <c r="AB46" s="9"/>
+    </row>
+    <row r="47" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="E47" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="AA47" s="4"/>
+      <c r="AB47" s="9"/>
+    </row>
+    <row r="48" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="51" t="s">
+      <c r="E48" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="AA48" s="4"/>
+      <c r="AB48" s="9"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="50" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="50" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="49"/>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" t="s">
+        <v>182</v>
+      </c>
+      <c r="E52" t="s">
+        <v>183</v>
+      </c>
+      <c r="F52" s="50"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="50" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" t="s">
+        <v>148</v>
+      </c>
+      <c r="E55" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="50" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>333</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -3564,11 +4147,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:DV89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3588,7 +4171,7 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
@@ -3604,10 +4187,10 @@
         <v>76</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="AA6" s="8"/>
       <c r="AB6" s="5"/>
@@ -3626,25 +4209,25 @@
         <v>80</v>
       </c>
       <c r="H9" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="I9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="AA9"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="B10">
         <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="I10" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="AA10"/>
     </row>
@@ -3656,10 +4239,10 @@
         <v>1.2E-2</v>
       </c>
       <c r="H11" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="I11" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="AA11"/>
     </row>
@@ -3671,10 +4254,10 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="H12" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="I12" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="AA12"/>
     </row>
@@ -3686,25 +4269,25 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="I13" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="AA13"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="I14" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="AA14"/>
     </row>
@@ -3716,10 +4299,10 @@
         <v>1.4</v>
       </c>
       <c r="H15" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I15" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="AA15"/>
     </row>
@@ -3732,7 +4315,7 @@
       </c>
       <c r="E16" s="13"/>
       <c r="I16" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="AA16"/>
     </row>
@@ -3744,7 +4327,7 @@
         <v>0.01</v>
       </c>
       <c r="I17" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="AA17"/>
     </row>
@@ -3753,7 +4336,7 @@
     </row>
     <row r="19" spans="1:103" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:103" x14ac:dyDescent="0.3">
@@ -3764,10 +4347,10 @@
         <v>60</v>
       </c>
       <c r="H20" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="I20" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="AA20"/>
     </row>
@@ -3779,7 +4362,7 @@
         <v>8</v>
       </c>
       <c r="I21" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="AB21" s="9"/>
       <c r="AZ21" s="4"/>
@@ -3791,7 +4374,7 @@
     </row>
     <row r="22" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="B22">
         <v>0.01</v>
@@ -3812,7 +4395,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="AB23" s="9"/>
       <c r="AZ23" s="4"/>
@@ -3830,7 +4413,7 @@
         <v>0.63959999999999995</v>
       </c>
       <c r="I24" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="AA24"/>
     </row>
@@ -3842,7 +4425,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I25" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="AB25" s="9"/>
       <c r="AZ25" s="4"/>
@@ -3872,7 +4455,7 @@
         <v>328</v>
       </c>
       <c r="I26" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="AZ26" s="4"/>
       <c r="BY26" s="4"/>
@@ -3880,21 +4463,21 @@
     </row>
     <row r="27" spans="1:103" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B28">
         <v>15</v>
       </c>
       <c r="H28" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="I28" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="AZ28" s="4"/>
       <c r="BY28" s="4"/>
@@ -3902,16 +4485,16 @@
     </row>
     <row r="29" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B29">
         <v>0.50700000000000001</v>
       </c>
       <c r="H29" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I29" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="AZ29" s="4"/>
       <c r="BY29" s="4"/>
@@ -3919,16 +4502,16 @@
     </row>
     <row r="30" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="I30" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="AZ30" s="4"/>
       <c r="BY30" s="4"/>
@@ -3936,16 +4519,16 @@
     </row>
     <row r="31" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I31" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="AZ31" s="4"/>
       <c r="BY31" s="4"/>
@@ -3953,13 +4536,13 @@
     </row>
     <row r="32" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="AZ32" s="4"/>
       <c r="BY32" s="4"/>
@@ -3988,7 +4571,7 @@
       </c>
       <c r="G35" s="13"/>
       <c r="I35" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="AB35" s="9"/>
       <c r="AZ35" s="4"/>
@@ -4020,7 +4603,7 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="AZ38" s="4"/>
       <c r="BY38" s="4"/>
@@ -4034,10 +4617,10 @@
         <v>500</v>
       </c>
       <c r="H39" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="I39" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="AZ39" s="4"/>
       <c r="BY39" s="4"/>
@@ -4051,7 +4634,7 @@
         <v>0.06</v>
       </c>
       <c r="I40" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="AZ40" s="4"/>
       <c r="BY40" s="4"/>
@@ -4065,10 +4648,10 @@
         <v>1180</v>
       </c>
       <c r="H41" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="I41" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="AZ41" s="4"/>
       <c r="BY41" s="4"/>
@@ -4082,10 +4665,10 @@
         <v>1800</v>
       </c>
       <c r="H42" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="I42" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="AZ42" s="4"/>
       <c r="BY42" s="4"/>
@@ -4099,10 +4682,10 @@
         <v>1.55</v>
       </c>
       <c r="H43" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="I43" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="AZ43" s="4"/>
       <c r="BY43" s="4"/>
@@ -4110,13 +4693,13 @@
     </row>
     <row r="44" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B44">
         <v>0.25</v>
       </c>
       <c r="I44" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="AZ44" s="4"/>
       <c r="BY44" s="4"/>
@@ -4124,13 +4707,13 @@
     </row>
     <row r="45" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="B45">
         <v>0.5</v>
       </c>
       <c r="I45" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="AZ45" s="4"/>
       <c r="BY45" s="4"/>
@@ -4138,13 +4721,13 @@
     </row>
     <row r="46" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="B46">
         <v>25</v>
       </c>
       <c r="I46" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="AZ46" s="4"/>
       <c r="BY46" s="4"/>
@@ -4152,13 +4735,13 @@
     </row>
     <row r="47" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="B47">
         <v>45</v>
       </c>
       <c r="I47" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="AZ47" s="4"/>
       <c r="BY47" s="4"/>
@@ -4185,23 +4768,11 @@
       <c r="B50" s="9">
         <v>3</v>
       </c>
-      <c r="C50">
-        <v>5</v>
-      </c>
-      <c r="D50">
-        <v>7</v>
-      </c>
-      <c r="E50">
-        <v>10</v>
-      </c>
-      <c r="F50">
-        <v>15</v>
-      </c>
       <c r="H50" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="I50" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="AB50" s="4"/>
       <c r="AC50" s="4"/>
@@ -4314,13 +4885,13 @@
         <v>17</v>
       </c>
       <c r="I51" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="AB51" s="9"/>
     </row>
     <row r="52" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B52">
         <v>-0.35</v>
@@ -4329,14 +4900,14 @@
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
       <c r="I52" s="11" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J52" s="11"/>
       <c r="AB52" s="9"/>
     </row>
     <row r="53" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B53">
         <v>-0.15</v>
@@ -4345,14 +4916,14 @@
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
       <c r="I53" s="11" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="J53" s="11"/>
       <c r="AB53" s="9"/>
     </row>
     <row r="54" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B54">
         <v>0.1</v>
@@ -4361,7 +4932,7 @@
         <v>17</v>
       </c>
       <c r="I54" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="AB54" s="9"/>
     </row>
@@ -4382,7 +4953,7 @@
         <v>17</v>
       </c>
       <c r="I57" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:126" x14ac:dyDescent="0.3">
@@ -4393,10 +4964,10 @@
         <v>600</v>
       </c>
       <c r="H58" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="I58" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:126" x14ac:dyDescent="0.3">
@@ -4407,10 +4978,10 @@
         <v>20</v>
       </c>
       <c r="H59" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="I59" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:126" x14ac:dyDescent="0.3">
@@ -4421,10 +4992,10 @@
         <v>300</v>
       </c>
       <c r="H60" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="I60" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:126" x14ac:dyDescent="0.3">
@@ -4435,10 +5006,10 @@
         <v>970</v>
       </c>
       <c r="H61" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="I61" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:126" x14ac:dyDescent="0.3">
@@ -4449,10 +5020,10 @@
         <v>15</v>
       </c>
       <c r="H62" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="I62" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:126" x14ac:dyDescent="0.3">
@@ -4463,10 +5034,10 @@
         <v>2</v>
       </c>
       <c r="H63" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="I63" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:126" x14ac:dyDescent="0.3">
@@ -4477,13 +5048,13 @@
         <v>380</v>
       </c>
       <c r="H64" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="I64" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="J64" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:28" x14ac:dyDescent="0.3">
@@ -4494,10 +5065,10 @@
         <v>209</v>
       </c>
       <c r="H65" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="I65" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="67" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4518,7 +5089,7 @@
         <v>17</v>
       </c>
       <c r="I68" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="AB68" s="9"/>
     </row>
@@ -4534,7 +5105,7 @@
         <v>17</v>
       </c>
       <c r="I69" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="AB69" s="9"/>
     </row>
@@ -4546,7 +5117,7 @@
         <v>0.3</v>
       </c>
       <c r="I70" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="AB70" s="9"/>
     </row>
@@ -4558,10 +5129,10 @@
         <v>10</v>
       </c>
       <c r="H71" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="I71" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="AB71" s="9"/>
     </row>
@@ -4573,7 +5144,7 @@
         <v>0.35</v>
       </c>
       <c r="I72" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="73" spans="1:28" x14ac:dyDescent="0.3">
@@ -4584,7 +5155,7 @@
         <v>20.6</v>
       </c>
       <c r="I73" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="74" spans="1:28" x14ac:dyDescent="0.3">
@@ -4595,7 +5166,7 @@
         <v>0.2</v>
       </c>
       <c r="I74" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" spans="1:28" x14ac:dyDescent="0.3">
@@ -4606,7 +5177,7 @@
         <v>0.01</v>
       </c>
       <c r="I75" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="76" spans="1:28" x14ac:dyDescent="0.3">
@@ -4617,10 +5188,10 @@
         <v>10</v>
       </c>
       <c r="H76" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="I76" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="77" spans="1:28" x14ac:dyDescent="0.3">
@@ -4631,10 +5202,10 @@
         <v>0</v>
       </c>
       <c r="H77" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="I77" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4648,10 +5219,10 @@
         <v>52</v>
       </c>
       <c r="B80" s="9">
-        <v>169</v>
+        <v>20060618</v>
       </c>
       <c r="I80" t="s">
-        <v>204</v>
+        <v>370</v>
       </c>
       <c r="AB80" s="9"/>
     </row>
@@ -4660,10 +5231,10 @@
         <v>53</v>
       </c>
       <c r="B81">
-        <v>170</v>
+        <v>20060619</v>
       </c>
       <c r="I81" t="s">
-        <v>205</v>
+        <v>371</v>
       </c>
       <c r="AB81" s="9"/>
     </row>
@@ -4675,10 +5246,10 @@
         <v>52.25</v>
       </c>
       <c r="H82" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="I82" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="AB82" s="9"/>
     </row>
@@ -4690,10 +5261,10 @@
         <v>5.69</v>
       </c>
       <c r="H83" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="I83" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="AB83" s="9"/>
     </row>
@@ -4705,60 +5276,60 @@
         <v>1</v>
       </c>
       <c r="H84" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="I84" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="86" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="AA86" s="7"/>
     </row>
     <row r="87" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B87" s="9">
         <v>30</v>
       </c>
       <c r="H87" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="I87" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="AB87" s="9"/>
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B88" s="9">
         <v>0</v>
       </c>
       <c r="H88" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="I88" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="AB88" s="9"/>
     </row>
     <row r="89" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B89" s="9">
         <v>90</v>
       </c>
       <c r="H89" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="I89" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="AB89" s="9"/>
     </row>

</xml_diff>

<commit_message>
date calculation from doy
</commit_message>
<xml_diff>
--- a/SCOPE_v1.73/input_data.xlsx
+++ b/SCOPE_v1.73/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm_projects\SCOPE-CvT\SCOPE_v1.73\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70689859-450B-4A3A-BC53-42295DFCA0ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B62C9CF-8AE5-4B43-8911-6982821DA28B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="378">
   <si>
     <t>Cab</t>
   </si>
@@ -1416,6 +1416,31 @@
   </si>
   <si>
     <t>Variables below are COLUMN NAMES in time_series_files (meteo_ec_csv, vegetation_retrieved_csv)</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>year [if t == DOY]</t>
+  </si>
+  <si>
+    <t>[OPTIONAL]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if t is DOY this will be used to convert it to date-time: however, startDOY, endDOY </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>must be timestamps</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3528,10 +3553,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:DV58"/>
+  <dimension ref="A1:DV59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3670,234 +3695,236 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>8</v>
+        <v>374</v>
       </c>
       <c r="D18" t="s">
-        <v>172</v>
+        <v>376</v>
       </c>
       <c r="E18" t="s">
-        <v>342</v>
+        <v>375</v>
+      </c>
+      <c r="F18" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
         <v>172</v>
       </c>
       <c r="E19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>339</v>
+        <v>172</v>
       </c>
       <c r="E20" t="s">
-        <v>178</v>
+        <v>343</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E21" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>180</v>
+        <v>340</v>
       </c>
       <c r="E22" t="s">
-        <v>344</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E23" t="s">
-        <v>347</v>
-      </c>
-      <c r="F23" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>177</v>
+      </c>
+      <c r="E24" t="s">
+        <v>347</v>
+      </c>
+      <c r="F24" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>335</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>341</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>356</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F25" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>95</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>201</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>202</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>0</v>
-      </c>
-      <c r="D30" t="s">
-        <v>136</v>
-      </c>
-      <c r="E30" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="48" t="s">
-        <v>309</v>
       </c>
       <c r="D31" t="s">
         <v>136</v>
       </c>
       <c r="E31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="48" t="s">
+        <v>309</v>
+      </c>
+      <c r="D32" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" t="s">
         <v>310</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s">
-        <v>138</v>
-      </c>
-      <c r="E32" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E33" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E34" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>319</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E35" t="s">
-        <v>320</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>319</v>
+      </c>
+      <c r="D36" t="s">
+        <v>136</v>
+      </c>
+      <c r="E36" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="37" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>6</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>144</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:126" x14ac:dyDescent="0.3">
-      <c r="A38" s="50" t="s">
+    <row r="39" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A39" s="50" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="39" spans="1:126" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" t="s">
-        <v>341</v>
-      </c>
-      <c r="E39" t="s">
-        <v>164</v>
-      </c>
-      <c r="F39" s="50"/>
-      <c r="AA39" s="4"/>
-      <c r="AZ39" s="4"/>
-      <c r="BY39" s="4"/>
-      <c r="CX39" s="4"/>
     </row>
     <row r="40" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>332</v>
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
+        <v>341</v>
       </c>
       <c r="E40" t="s">
-        <v>329</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="F40" s="50"/>
       <c r="AA40" s="4"/>
       <c r="AZ40" s="4"/>
       <c r="BY40" s="4"/>
@@ -3905,10 +3932,10 @@
     </row>
     <row r="41" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="E41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AA41" s="4"/>
       <c r="AZ41" s="4"/>
@@ -3917,166 +3944,164 @@
     </row>
     <row r="42" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E42" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AA42" s="4"/>
       <c r="AZ42" s="4"/>
       <c r="BY42" s="4"/>
       <c r="CX42" s="4"/>
     </row>
-    <row r="44" spans="1:126" s="52" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="51" t="s">
+    <row r="43" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>328</v>
+      </c>
+      <c r="E43" t="s">
+        <v>331</v>
+      </c>
+      <c r="AA43" s="4"/>
+      <c r="AZ43" s="4"/>
+      <c r="BY43" s="4"/>
+      <c r="CX43" s="4"/>
+    </row>
+    <row r="45" spans="1:126" s="52" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="51" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:126" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="9"/>
-      <c r="D45" t="s">
-        <v>165</v>
-      </c>
-      <c r="E45" t="s">
-        <v>166</v>
-      </c>
-      <c r="AA45" s="4"/>
-      <c r="AB45" s="4"/>
-      <c r="AC45" s="4"/>
-      <c r="AD45" s="4"/>
-      <c r="AE45" s="4"/>
-      <c r="AF45" s="4"/>
-      <c r="AG45" s="4"/>
-      <c r="AH45" s="4"/>
-      <c r="AI45" s="4"/>
-      <c r="AJ45" s="4"/>
-      <c r="AK45" s="4"/>
-      <c r="AL45" s="4"/>
-      <c r="AM45" s="4"/>
-      <c r="AN45" s="4"/>
-      <c r="AO45" s="4"/>
-      <c r="AP45" s="4"/>
-      <c r="AQ45" s="4"/>
-      <c r="AR45" s="4"/>
-      <c r="AS45" s="4"/>
-      <c r="AT45" s="4"/>
-      <c r="AU45" s="4"/>
-      <c r="AV45" s="4"/>
-      <c r="AW45" s="4"/>
-      <c r="AX45" s="4"/>
-      <c r="AY45" s="4"/>
-      <c r="AZ45" s="4"/>
-      <c r="BA45" s="4"/>
-      <c r="BB45" s="4"/>
-      <c r="BC45" s="4"/>
-      <c r="BD45" s="4"/>
-      <c r="BE45" s="4"/>
-      <c r="BF45" s="4"/>
-      <c r="BG45" s="4"/>
-      <c r="BH45" s="4"/>
-      <c r="BI45" s="4"/>
-      <c r="BJ45" s="4"/>
-      <c r="BK45" s="4"/>
-      <c r="BL45" s="4"/>
-      <c r="BM45" s="4"/>
-      <c r="BN45" s="4"/>
-      <c r="BO45" s="4"/>
-      <c r="BP45" s="4"/>
-      <c r="BQ45" s="4"/>
-      <c r="BR45" s="4"/>
-      <c r="BS45" s="4"/>
-      <c r="BT45" s="4"/>
-      <c r="BU45" s="4"/>
-      <c r="BV45" s="4"/>
-      <c r="BW45" s="4"/>
-      <c r="BX45" s="4"/>
-      <c r="BY45" s="4"/>
-      <c r="BZ45" s="4"/>
-      <c r="CA45" s="4"/>
-      <c r="CB45" s="4"/>
-      <c r="CC45" s="4"/>
-      <c r="CD45" s="4"/>
-      <c r="CE45" s="4"/>
-      <c r="CF45" s="4"/>
-      <c r="CG45" s="4"/>
-      <c r="CH45" s="4"/>
-      <c r="CI45" s="4"/>
-      <c r="CJ45" s="4"/>
-      <c r="CK45" s="4"/>
-      <c r="CL45" s="4"/>
-      <c r="CM45" s="4"/>
-      <c r="CN45" s="4"/>
-      <c r="CO45" s="4"/>
-      <c r="CP45" s="4"/>
-      <c r="CQ45" s="4"/>
-      <c r="CR45" s="4"/>
-      <c r="CS45" s="4"/>
-      <c r="CT45" s="4"/>
-      <c r="CU45" s="4"/>
-      <c r="CV45" s="4"/>
-      <c r="CW45" s="4"/>
-      <c r="CX45" s="4"/>
-      <c r="CY45" s="4"/>
-      <c r="CZ45" s="4"/>
-      <c r="DA45" s="4"/>
-      <c r="DB45" s="4"/>
-      <c r="DC45" s="4"/>
-      <c r="DD45" s="4"/>
-      <c r="DE45" s="4"/>
-      <c r="DF45" s="4"/>
-      <c r="DG45" s="4"/>
-      <c r="DH45" s="4"/>
-      <c r="DI45" s="4"/>
-      <c r="DJ45" s="4"/>
-      <c r="DK45" s="4"/>
-      <c r="DL45" s="4"/>
-      <c r="DM45" s="4"/>
-      <c r="DN45" s="4"/>
-      <c r="DO45" s="4"/>
-      <c r="DP45" s="4"/>
-      <c r="DQ45" s="4"/>
-      <c r="DR45" s="4"/>
-      <c r="DS45" s="4"/>
-      <c r="DT45" s="4"/>
-      <c r="DU45" s="4"/>
-      <c r="DV45" s="4"/>
     </row>
     <row r="46" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>24</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B46" s="9"/>
       <c r="D46" t="s">
-        <v>17</v>
+        <v>165</v>
       </c>
       <c r="E46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AA46" s="4"/>
-      <c r="AB46" s="9"/>
+      <c r="AB46" s="4"/>
+      <c r="AC46" s="4"/>
+      <c r="AD46" s="4"/>
+      <c r="AE46" s="4"/>
+      <c r="AF46" s="4"/>
+      <c r="AG46" s="4"/>
+      <c r="AH46" s="4"/>
+      <c r="AI46" s="4"/>
+      <c r="AJ46" s="4"/>
+      <c r="AK46" s="4"/>
+      <c r="AL46" s="4"/>
+      <c r="AM46" s="4"/>
+      <c r="AN46" s="4"/>
+      <c r="AO46" s="4"/>
+      <c r="AP46" s="4"/>
+      <c r="AQ46" s="4"/>
+      <c r="AR46" s="4"/>
+      <c r="AS46" s="4"/>
+      <c r="AT46" s="4"/>
+      <c r="AU46" s="4"/>
+      <c r="AV46" s="4"/>
+      <c r="AW46" s="4"/>
+      <c r="AX46" s="4"/>
+      <c r="AY46" s="4"/>
+      <c r="AZ46" s="4"/>
+      <c r="BA46" s="4"/>
+      <c r="BB46" s="4"/>
+      <c r="BC46" s="4"/>
+      <c r="BD46" s="4"/>
+      <c r="BE46" s="4"/>
+      <c r="BF46" s="4"/>
+      <c r="BG46" s="4"/>
+      <c r="BH46" s="4"/>
+      <c r="BI46" s="4"/>
+      <c r="BJ46" s="4"/>
+      <c r="BK46" s="4"/>
+      <c r="BL46" s="4"/>
+      <c r="BM46" s="4"/>
+      <c r="BN46" s="4"/>
+      <c r="BO46" s="4"/>
+      <c r="BP46" s="4"/>
+      <c r="BQ46" s="4"/>
+      <c r="BR46" s="4"/>
+      <c r="BS46" s="4"/>
+      <c r="BT46" s="4"/>
+      <c r="BU46" s="4"/>
+      <c r="BV46" s="4"/>
+      <c r="BW46" s="4"/>
+      <c r="BX46" s="4"/>
+      <c r="BY46" s="4"/>
+      <c r="BZ46" s="4"/>
+      <c r="CA46" s="4"/>
+      <c r="CB46" s="4"/>
+      <c r="CC46" s="4"/>
+      <c r="CD46" s="4"/>
+      <c r="CE46" s="4"/>
+      <c r="CF46" s="4"/>
+      <c r="CG46" s="4"/>
+      <c r="CH46" s="4"/>
+      <c r="CI46" s="4"/>
+      <c r="CJ46" s="4"/>
+      <c r="CK46" s="4"/>
+      <c r="CL46" s="4"/>
+      <c r="CM46" s="4"/>
+      <c r="CN46" s="4"/>
+      <c r="CO46" s="4"/>
+      <c r="CP46" s="4"/>
+      <c r="CQ46" s="4"/>
+      <c r="CR46" s="4"/>
+      <c r="CS46" s="4"/>
+      <c r="CT46" s="4"/>
+      <c r="CU46" s="4"/>
+      <c r="CV46" s="4"/>
+      <c r="CW46" s="4"/>
+      <c r="CX46" s="4"/>
+      <c r="CY46" s="4"/>
+      <c r="CZ46" s="4"/>
+      <c r="DA46" s="4"/>
+      <c r="DB46" s="4"/>
+      <c r="DC46" s="4"/>
+      <c r="DD46" s="4"/>
+      <c r="DE46" s="4"/>
+      <c r="DF46" s="4"/>
+      <c r="DG46" s="4"/>
+      <c r="DH46" s="4"/>
+      <c r="DI46" s="4"/>
+      <c r="DJ46" s="4"/>
+      <c r="DK46" s="4"/>
+      <c r="DL46" s="4"/>
+      <c r="DM46" s="4"/>
+      <c r="DN46" s="4"/>
+      <c r="DO46" s="4"/>
+      <c r="DP46" s="4"/>
+      <c r="DQ46" s="4"/>
+      <c r="DR46" s="4"/>
+      <c r="DS46" s="4"/>
+      <c r="DT46" s="4"/>
+      <c r="DU46" s="4"/>
+      <c r="DV46" s="4"/>
     </row>
     <row r="47" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>100</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="D47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" t="s">
+        <v>167</v>
+      </c>
       <c r="AA47" s="4"/>
       <c r="AB47" s="9"/>
     </row>
     <row r="48" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
@@ -4085,57 +4110,71 @@
       <c r="AA48" s="4"/>
       <c r="AB48" s="9"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="50" t="s">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="AA49" s="4"/>
+      <c r="AB49" s="9"/>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A51" s="50" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>7</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>17</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E52" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>14</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>182</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" t="s">
         <v>183</v>
       </c>
-      <c r="F52" s="50"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="50" t="s">
+      <c r="F53" s="50"/>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A55" s="50" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>16</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>148</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E56" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="50" t="s">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A58" s="50" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>333</v>
       </c>
     </row>
@@ -4150,7 +4189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:DV89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ebal errors catching - NaN writing, csv output
</commit_message>
<xml_diff>
--- a/SCOPE_v1.73/input_data.xlsx
+++ b/SCOPE_v1.73/input_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm_projects\SCOPE-CvT\SCOPE_v1.73\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B62C9CF-8AE5-4B43-8911-6982821DA28B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2018135B-71B9-4CC9-899B-07CC7773C020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="380">
   <si>
     <t>Cab</t>
   </si>
@@ -1283,9 +1283,6 @@
     <t>atmospherc vapor pressure</t>
   </si>
   <si>
-    <t>if not present - calculated from RH_file: RH * satvap(Ta)</t>
-  </si>
-  <si>
     <t>definition</t>
   </si>
   <si>
@@ -1305,9 +1302,6 @@
   </si>
   <si>
     <t>Leaf</t>
-  </si>
-  <si>
-    <t>relative humidity (for calculation of ea)</t>
   </si>
   <si>
     <t>optiona_leaf_inclination_distribution_dat_file_with_13_rows_(probability_histogram)._MUST_be_located_in_../data/leafangles/</t>
@@ -1351,9 +1345,6 @@
   </si>
   <si>
     <t>verification_run</t>
-  </si>
-  <si>
-    <t>verificationdata</t>
   </si>
   <si>
     <t>f_date</t>
@@ -1441,6 +1432,21 @@
       </rPr>
       <t>must be timestamps</t>
     </r>
+  </si>
+  <si>
+    <t>verificationdata_csv</t>
+  </si>
+  <si>
+    <t>VPD</t>
+  </si>
+  <si>
+    <t>vapour pressure deficit</t>
+  </si>
+  <si>
+    <t>relative humidity</t>
+  </si>
+  <si>
+    <t>if not present - calculated from air temperature (Ta) and RH: RH * satvap(Ta) or VPD: satvap(Ta) - VPD</t>
   </si>
 </sst>
 </file>
@@ -3553,10 +3559,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:DV59"/>
+  <dimension ref="A1:DV60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3585,7 +3591,7 @@
         <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -3626,57 +3632,57 @@
         <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>356</v>
+      </c>
+      <c r="B11" t="s">
+        <v>375</v>
+      </c>
+      <c r="D11" t="s">
         <v>358</v>
-      </c>
-      <c r="B11" t="s">
-        <v>367</v>
-      </c>
-      <c r="D11" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B12" t="s">
         <v>336</v>
       </c>
       <c r="D12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E12" s="50"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D14" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D16" t="s">
         <v>338</v>
       </c>
       <c r="E16" t="s">
+        <v>348</v>
+      </c>
+      <c r="F16" t="s">
         <v>349</v>
-      </c>
-      <c r="F16" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -3684,10 +3690,10 @@
         <v>337</v>
       </c>
       <c r="B17" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E17" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F17" t="s">
         <v>334</v>
@@ -3695,16 +3701,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>371</v>
+      </c>
+      <c r="D18" t="s">
+        <v>373</v>
+      </c>
+      <c r="E18" t="s">
+        <v>372</v>
+      </c>
+      <c r="F18" t="s">
         <v>374</v>
-      </c>
-      <c r="D18" t="s">
-        <v>376</v>
-      </c>
-      <c r="E18" t="s">
-        <v>375</v>
-      </c>
-      <c r="F18" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -3791,7 +3797,7 @@
         <v>347</v>
       </c>
       <c r="F24" t="s">
-        <v>348</v>
+        <v>379</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3802,141 +3808,143 @@
         <v>341</v>
       </c>
       <c r="E25" t="s">
-        <v>356</v>
+        <v>378</v>
       </c>
       <c r="F25" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>376</v>
+      </c>
+      <c r="D26" t="s">
+        <v>177</v>
+      </c>
+      <c r="E26" t="s">
+        <v>377</v>
+      </c>
+      <c r="F26" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>95</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>201</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>202</v>
       </c>
-      <c r="F27" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="F28" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
-        <v>355</v>
-      </c>
-    </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>0</v>
-      </c>
-      <c r="D31" t="s">
-        <v>136</v>
-      </c>
-      <c r="E31" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="48" t="s">
-        <v>309</v>
       </c>
       <c r="D32" t="s">
         <v>136</v>
       </c>
       <c r="E32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A33" s="48" t="s">
+        <v>309</v>
+      </c>
+      <c r="D33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
         <v>310</v>
-      </c>
-    </row>
-    <row r="33" spans="1:126" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" t="s">
-        <v>138</v>
-      </c>
-      <c r="E33" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E34" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>319</v>
+        <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E36" t="s">
-        <v>320</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>319</v>
+      </c>
+      <c r="D37" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="38" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>6</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>144</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:126" x14ac:dyDescent="0.3">
-      <c r="A39" s="50" t="s">
-        <v>352</v>
-      </c>
-    </row>
     <row r="40" spans="1:126" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>98</v>
-      </c>
-      <c r="D40" t="s">
-        <v>341</v>
-      </c>
-      <c r="E40" t="s">
-        <v>164</v>
-      </c>
-      <c r="F40" s="50"/>
-      <c r="AA40" s="4"/>
-      <c r="AZ40" s="4"/>
-      <c r="BY40" s="4"/>
-      <c r="CX40" s="4"/>
+      <c r="A40" s="50" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="41" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>332</v>
+        <v>98</v>
+      </c>
+      <c r="D41" t="s">
+        <v>341</v>
       </c>
       <c r="E41" t="s">
-        <v>329</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="F41" s="50"/>
       <c r="AA41" s="4"/>
       <c r="AZ41" s="4"/>
       <c r="BY41" s="4"/>
@@ -3944,10 +3952,10 @@
     </row>
     <row r="42" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="E42" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AA42" s="4"/>
       <c r="AZ42" s="4"/>
@@ -3956,166 +3964,164 @@
     </row>
     <row r="43" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E43" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AA43" s="4"/>
       <c r="AZ43" s="4"/>
       <c r="BY43" s="4"/>
       <c r="CX43" s="4"/>
     </row>
-    <row r="45" spans="1:126" s="52" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="51" t="s">
+    <row r="44" spans="1:126" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>328</v>
+      </c>
+      <c r="E44" t="s">
+        <v>331</v>
+      </c>
+      <c r="AA44" s="4"/>
+      <c r="AZ44" s="4"/>
+      <c r="BY44" s="4"/>
+      <c r="CX44" s="4"/>
+    </row>
+    <row r="46" spans="1:126" s="52" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="51" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:126" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="9"/>
-      <c r="D46" t="s">
-        <v>165</v>
-      </c>
-      <c r="E46" t="s">
-        <v>166</v>
-      </c>
-      <c r="AA46" s="4"/>
-      <c r="AB46" s="4"/>
-      <c r="AC46" s="4"/>
-      <c r="AD46" s="4"/>
-      <c r="AE46" s="4"/>
-      <c r="AF46" s="4"/>
-      <c r="AG46" s="4"/>
-      <c r="AH46" s="4"/>
-      <c r="AI46" s="4"/>
-      <c r="AJ46" s="4"/>
-      <c r="AK46" s="4"/>
-      <c r="AL46" s="4"/>
-      <c r="AM46" s="4"/>
-      <c r="AN46" s="4"/>
-      <c r="AO46" s="4"/>
-      <c r="AP46" s="4"/>
-      <c r="AQ46" s="4"/>
-      <c r="AR46" s="4"/>
-      <c r="AS46" s="4"/>
-      <c r="AT46" s="4"/>
-      <c r="AU46" s="4"/>
-      <c r="AV46" s="4"/>
-      <c r="AW46" s="4"/>
-      <c r="AX46" s="4"/>
-      <c r="AY46" s="4"/>
-      <c r="AZ46" s="4"/>
-      <c r="BA46" s="4"/>
-      <c r="BB46" s="4"/>
-      <c r="BC46" s="4"/>
-      <c r="BD46" s="4"/>
-      <c r="BE46" s="4"/>
-      <c r="BF46" s="4"/>
-      <c r="BG46" s="4"/>
-      <c r="BH46" s="4"/>
-      <c r="BI46" s="4"/>
-      <c r="BJ46" s="4"/>
-      <c r="BK46" s="4"/>
-      <c r="BL46" s="4"/>
-      <c r="BM46" s="4"/>
-      <c r="BN46" s="4"/>
-      <c r="BO46" s="4"/>
-      <c r="BP46" s="4"/>
-      <c r="BQ46" s="4"/>
-      <c r="BR46" s="4"/>
-      <c r="BS46" s="4"/>
-      <c r="BT46" s="4"/>
-      <c r="BU46" s="4"/>
-      <c r="BV46" s="4"/>
-      <c r="BW46" s="4"/>
-      <c r="BX46" s="4"/>
-      <c r="BY46" s="4"/>
-      <c r="BZ46" s="4"/>
-      <c r="CA46" s="4"/>
-      <c r="CB46" s="4"/>
-      <c r="CC46" s="4"/>
-      <c r="CD46" s="4"/>
-      <c r="CE46" s="4"/>
-      <c r="CF46" s="4"/>
-      <c r="CG46" s="4"/>
-      <c r="CH46" s="4"/>
-      <c r="CI46" s="4"/>
-      <c r="CJ46" s="4"/>
-      <c r="CK46" s="4"/>
-      <c r="CL46" s="4"/>
-      <c r="CM46" s="4"/>
-      <c r="CN46" s="4"/>
-      <c r="CO46" s="4"/>
-      <c r="CP46" s="4"/>
-      <c r="CQ46" s="4"/>
-      <c r="CR46" s="4"/>
-      <c r="CS46" s="4"/>
-      <c r="CT46" s="4"/>
-      <c r="CU46" s="4"/>
-      <c r="CV46" s="4"/>
-      <c r="CW46" s="4"/>
-      <c r="CX46" s="4"/>
-      <c r="CY46" s="4"/>
-      <c r="CZ46" s="4"/>
-      <c r="DA46" s="4"/>
-      <c r="DB46" s="4"/>
-      <c r="DC46" s="4"/>
-      <c r="DD46" s="4"/>
-      <c r="DE46" s="4"/>
-      <c r="DF46" s="4"/>
-      <c r="DG46" s="4"/>
-      <c r="DH46" s="4"/>
-      <c r="DI46" s="4"/>
-      <c r="DJ46" s="4"/>
-      <c r="DK46" s="4"/>
-      <c r="DL46" s="4"/>
-      <c r="DM46" s="4"/>
-      <c r="DN46" s="4"/>
-      <c r="DO46" s="4"/>
-      <c r="DP46" s="4"/>
-      <c r="DQ46" s="4"/>
-      <c r="DR46" s="4"/>
-      <c r="DS46" s="4"/>
-      <c r="DT46" s="4"/>
-      <c r="DU46" s="4"/>
-      <c r="DV46" s="4"/>
     </row>
     <row r="47" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>24</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B47" s="9"/>
       <c r="D47" t="s">
-        <v>17</v>
+        <v>165</v>
       </c>
       <c r="E47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AA47" s="4"/>
-      <c r="AB47" s="9"/>
+      <c r="AB47" s="4"/>
+      <c r="AC47" s="4"/>
+      <c r="AD47" s="4"/>
+      <c r="AE47" s="4"/>
+      <c r="AF47" s="4"/>
+      <c r="AG47" s="4"/>
+      <c r="AH47" s="4"/>
+      <c r="AI47" s="4"/>
+      <c r="AJ47" s="4"/>
+      <c r="AK47" s="4"/>
+      <c r="AL47" s="4"/>
+      <c r="AM47" s="4"/>
+      <c r="AN47" s="4"/>
+      <c r="AO47" s="4"/>
+      <c r="AP47" s="4"/>
+      <c r="AQ47" s="4"/>
+      <c r="AR47" s="4"/>
+      <c r="AS47" s="4"/>
+      <c r="AT47" s="4"/>
+      <c r="AU47" s="4"/>
+      <c r="AV47" s="4"/>
+      <c r="AW47" s="4"/>
+      <c r="AX47" s="4"/>
+      <c r="AY47" s="4"/>
+      <c r="AZ47" s="4"/>
+      <c r="BA47" s="4"/>
+      <c r="BB47" s="4"/>
+      <c r="BC47" s="4"/>
+      <c r="BD47" s="4"/>
+      <c r="BE47" s="4"/>
+      <c r="BF47" s="4"/>
+      <c r="BG47" s="4"/>
+      <c r="BH47" s="4"/>
+      <c r="BI47" s="4"/>
+      <c r="BJ47" s="4"/>
+      <c r="BK47" s="4"/>
+      <c r="BL47" s="4"/>
+      <c r="BM47" s="4"/>
+      <c r="BN47" s="4"/>
+      <c r="BO47" s="4"/>
+      <c r="BP47" s="4"/>
+      <c r="BQ47" s="4"/>
+      <c r="BR47" s="4"/>
+      <c r="BS47" s="4"/>
+      <c r="BT47" s="4"/>
+      <c r="BU47" s="4"/>
+      <c r="BV47" s="4"/>
+      <c r="BW47" s="4"/>
+      <c r="BX47" s="4"/>
+      <c r="BY47" s="4"/>
+      <c r="BZ47" s="4"/>
+      <c r="CA47" s="4"/>
+      <c r="CB47" s="4"/>
+      <c r="CC47" s="4"/>
+      <c r="CD47" s="4"/>
+      <c r="CE47" s="4"/>
+      <c r="CF47" s="4"/>
+      <c r="CG47" s="4"/>
+      <c r="CH47" s="4"/>
+      <c r="CI47" s="4"/>
+      <c r="CJ47" s="4"/>
+      <c r="CK47" s="4"/>
+      <c r="CL47" s="4"/>
+      <c r="CM47" s="4"/>
+      <c r="CN47" s="4"/>
+      <c r="CO47" s="4"/>
+      <c r="CP47" s="4"/>
+      <c r="CQ47" s="4"/>
+      <c r="CR47" s="4"/>
+      <c r="CS47" s="4"/>
+      <c r="CT47" s="4"/>
+      <c r="CU47" s="4"/>
+      <c r="CV47" s="4"/>
+      <c r="CW47" s="4"/>
+      <c r="CX47" s="4"/>
+      <c r="CY47" s="4"/>
+      <c r="CZ47" s="4"/>
+      <c r="DA47" s="4"/>
+      <c r="DB47" s="4"/>
+      <c r="DC47" s="4"/>
+      <c r="DD47" s="4"/>
+      <c r="DE47" s="4"/>
+      <c r="DF47" s="4"/>
+      <c r="DG47" s="4"/>
+      <c r="DH47" s="4"/>
+      <c r="DI47" s="4"/>
+      <c r="DJ47" s="4"/>
+      <c r="DK47" s="4"/>
+      <c r="DL47" s="4"/>
+      <c r="DM47" s="4"/>
+      <c r="DN47" s="4"/>
+      <c r="DO47" s="4"/>
+      <c r="DP47" s="4"/>
+      <c r="DQ47" s="4"/>
+      <c r="DR47" s="4"/>
+      <c r="DS47" s="4"/>
+      <c r="DT47" s="4"/>
+      <c r="DU47" s="4"/>
+      <c r="DV47" s="4"/>
     </row>
     <row r="48" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>100</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="D48" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" t="s">
+        <v>167</v>
+      </c>
       <c r="AA48" s="4"/>
       <c r="AB48" s="9"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
@@ -4124,57 +4130,71 @@
       <c r="AA49" s="4"/>
       <c r="AB49" s="9"/>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A51" s="50" t="s">
-        <v>353</v>
-      </c>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="AA50" s="4"/>
+      <c r="AB50" s="9"/>
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" t="s">
-        <v>17</v>
-      </c>
-      <c r="E52" t="s">
-        <v>345</v>
+      <c r="A52" s="50" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>14</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>182</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E54" t="s">
         <v>183</v>
       </c>
-      <c r="F53" s="50"/>
-    </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A55" s="50" t="s">
-        <v>354</v>
-      </c>
+      <c r="F54" s="50"/>
     </row>
     <row r="56" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="A56" s="50" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>16</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>148</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E57" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A58" s="50" t="s">
-        <v>357</v>
-      </c>
-    </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="A59" s="50" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>333</v>
       </c>
     </row>
@@ -5261,7 +5281,7 @@
         <v>20060618</v>
       </c>
       <c r="I80" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AB80" s="9"/>
     </row>
@@ -5273,7 +5293,7 @@
         <v>20060619</v>
       </c>
       <c r="I81" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AB81" s="9"/>
     </row>

</xml_diff>

<commit_message>
xlsx as input_csv for saving
</commit_message>
<xml_diff>
--- a/SCOPE_v1.73/input_data.xlsx
+++ b/SCOPE_v1.73/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm_projects\SCOPE-CvT\SCOPE_v1.73\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2018135B-71B9-4CC9-899B-07CC7773C020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4140F49F-CE6A-440B-94DE-15297F2D3DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="10044" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -1247,9 +1247,6 @@
     <t>RH</t>
   </si>
   <si>
-    <t>ts_input.csv</t>
-  </si>
-  <si>
     <t>t</t>
   </si>
   <si>
@@ -1287,9 +1284,6 @@
   </si>
   <si>
     <t>comment</t>
-  </si>
-  <si>
-    <t>missing values are -9999, NA or N/A</t>
   </si>
   <si>
     <t>BSM</t>
@@ -1447,6 +1441,25 @@
   </si>
   <si>
     <t>if not present - calculated from air temperature (Ta) and RH: RH * satvap(Ta) or VPD: satvap(Ta) - VPD</t>
+  </si>
+  <si>
+    <t>ts_input.xlsx</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">missing values are -9999, NA or N/A: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>excel does not save long integers (TIMESTAMP) in .csv properly =&gt; save as .xlsx if you change the input</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3562,7 +3575,7 @@
   <dimension ref="A1:DV60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3591,7 +3604,7 @@
         <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -3632,68 +3645,68 @@
         <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B11" t="s">
+        <v>373</v>
+      </c>
+      <c r="D11" t="s">
         <v>356</v>
-      </c>
-      <c r="B11" t="s">
-        <v>375</v>
-      </c>
-      <c r="D11" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B12" t="s">
-        <v>336</v>
+        <v>378</v>
       </c>
       <c r="D12" t="s">
-        <v>350</v>
+        <v>379</v>
       </c>
       <c r="E12" s="50"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E16" t="s">
+        <v>347</v>
+      </c>
+      <c r="F16" t="s">
         <v>348</v>
-      </c>
-      <c r="F16" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B17" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E17" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F17" t="s">
         <v>334</v>
@@ -3701,16 +3714,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>369</v>
+      </c>
+      <c r="D18" t="s">
         <v>371</v>
       </c>
-      <c r="D18" t="s">
-        <v>373</v>
-      </c>
       <c r="E18" t="s">
+        <v>370</v>
+      </c>
+      <c r="F18" t="s">
         <v>372</v>
-      </c>
-      <c r="F18" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -3724,7 +3737,7 @@
         <v>172</v>
       </c>
       <c r="E19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -3738,7 +3751,7 @@
         <v>172</v>
       </c>
       <c r="E20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3749,7 +3762,7 @@
         <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E21" t="s">
         <v>178</v>
@@ -3763,7 +3776,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E22" t="s">
         <v>175</v>
@@ -3780,7 +3793,7 @@
         <v>180</v>
       </c>
       <c r="E23" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -3794,10 +3807,10 @@
         <v>177</v>
       </c>
       <c r="E24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F24" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3805,27 +3818,27 @@
         <v>335</v>
       </c>
       <c r="D25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E25" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F25" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D26" t="s">
         <v>177</v>
       </c>
       <c r="E26" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F26" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -3839,7 +3852,7 @@
         <v>202</v>
       </c>
       <c r="F28" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -3849,7 +3862,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -3931,7 +3944,7 @@
     </row>
     <row r="40" spans="1:126" x14ac:dyDescent="0.3">
       <c r="A40" s="50" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="41" spans="1:126" x14ac:dyDescent="0.3">
@@ -3939,7 +3952,7 @@
         <v>98</v>
       </c>
       <c r="D41" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E41" t="s">
         <v>164</v>
@@ -4146,7 +4159,7 @@
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A52" s="50" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.3">
@@ -4157,7 +4170,7 @@
         <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.3">
@@ -4174,7 +4187,7 @@
     </row>
     <row r="56" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A56" s="50" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="57" spans="1:28" x14ac:dyDescent="0.3">
@@ -4185,12 +4198,12 @@
         <v>148</v>
       </c>
       <c r="E57" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A59" s="50" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.3">
@@ -5281,7 +5294,7 @@
         <v>20060618</v>
       </c>
       <c r="I80" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="AB80" s="9"/>
     </row>
@@ -5293,7 +5306,7 @@
         <v>20060619</v>
       </c>
       <c r="I81" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="AB81" s="9"/>
     </row>

</xml_diff>